<commit_message>
Added USB UART Schematic
</commit_message>
<xml_diff>
--- a/BT Mesh/Project Outputs for BT Mesh/BT Mesh.xlsx
+++ b/BT Mesh/Project Outputs for BT Mesh/BT Mesh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Preshit\Documents\GitHub\Low-Power-Embedded-Design\BT Mesh\Project Outputs for BT Mesh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{80CE4F55-E553-4BA3-9166-74B041F49001}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2FCB981C-BA98-4B5B-A32A-23469D590542}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{E0B52E10-F990-4D38-B944-E95D9B41FE75}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{1D8F6CD8-5044-47FF-A010-CF7A57ACA4F7}"/>
   </bookViews>
   <sheets>
     <sheet name="BT Mesh" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="332">
   <si>
     <t>Designator</t>
   </si>
@@ -87,28 +87,28 @@
     <t>SMTU2450N-LF BULK</t>
   </si>
   <si>
-    <t>C1, C6, C10, C16, C17</t>
+    <t>C1, C6, C10, C16, C17, C22, C23</t>
   </si>
   <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 25V X7R 0603, CAP CER 1UF 16V X7R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 1UF 25V X5R 0603</t>
+    <t>CAP CER 0.1UF 25V X7R 0603, CAP CER 1UF 16V X7R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 0.1UF 25V X7R 0603, CAP CER 0.1UF 25V X7R 0603</t>
   </si>
   <si>
     <t>Digi-Key Link</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM188R71E104KA57D/490-6051-1-ND/3845251, https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B105MO8NNWC/1276-6524-1-ND/5961383, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023</t>
-  </si>
-  <si>
-    <t>490-6051-1-ND, 1276-6524-1-ND, 490-12322-1-ND, 490-12322-1-ND, 490-12322-1-ND</t>
-  </si>
-  <si>
-    <t>Murata Electronics North America, Samsung Electro-Mechanics, Murata Electronics North America, Murata Electronics North America, Murata Electronics North America</t>
-  </si>
-  <si>
-    <t>GCM188R71E104KA57D, CL10B105MO8NNWC, GRT188R61E105ME13D, GRT188R61E105ME13D, GRT188R61E105ME13D</t>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM188R71E104KA57D/490-6051-1-ND/3845251, https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B105MO8NNWC/1276-6524-1-ND/5961383, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM188R71E104KA57D/490-6051-1-ND/3845251, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM188R71E104KA57D/490-6051-1-ND/3845251</t>
+  </si>
+  <si>
+    <t>490-6051-1-ND, 1276-6524-1-ND, 490-12322-1-ND, 490-12322-1-ND, 490-12322-1-ND, 490-6051-1-ND, 490-6051-1-ND</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America, Samsung Electro-Mechanics, Murata Electronics North America, Murata Electronics North America, Murata Electronics North America, Murata Electronics North America, Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>GCM188R71E104KA57D, CL10B105MO8NNWC, GRT188R61E105ME13D, GRT188R61E105ME13D, GRT188R61E105ME13D, GCM188R71E104KA57D, GCM188R71E104KA57D</t>
   </si>
   <si>
     <t>C2, C3, C5, C8, C15</t>
@@ -117,19 +117,19 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>CAP CER 10UF 25V X5R 1206, CAP CER 10UF 6.3V X5R 0603, CAP CER 10UF 6.3V X5R 0603, CAP CER 10UF 6.3V X5R 0603, CAP CER 10UF 6.3V X5R 0603</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GJ831CR61E106KE83L/490-14441-1-ND/6606902, https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10A106KQ8NNNC/1276-1038-1-ND/3889124, https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10A106KQ8NNNC/1276-1038-1-ND/3889124, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM188R60J106ME84D/490-7316-1-ND/4251709, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM188R60J106ME84D/490-7316-1-ND/4251709</t>
-  </si>
-  <si>
-    <t>490-14441-1-ND, 1276-1038-1-ND, 1276-1038-1-ND, 490-7316-1-ND, 490-7316-1-ND</t>
-  </si>
-  <si>
-    <t>Murata Electronics North America, Samsung Electro-Mechanics, Samsung Electro-Mechanics, Murata Electronics North America, Murata Electronics North America</t>
-  </si>
-  <si>
-    <t>GJ831CR61E106KE83L, CL10A106KQ8NNNC, CL10A106KQ8NNNC, GRM188R60J106ME84D, GRM188R60J106ME84D</t>
+    <t>CAP CER 10UF 10V X5R 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=490-10474-1-ND</t>
+  </si>
+  <si>
+    <t>490-10474-1-ND</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>GRM188R61A106KE69D</t>
   </si>
   <si>
     <t>C4</t>
@@ -159,10 +159,19 @@
     <t>10nF</t>
   </si>
   <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>C9</t>
+    <t>CAP CER 10000PF 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/kemet/C0603S103K4RACTU/399-9135-1-ND/3522653</t>
+  </si>
+  <si>
+    <t>399-9135-1-ND</t>
+  </si>
+  <si>
+    <t>C0603S103K4RACTU</t>
+  </si>
+  <si>
+    <t>C9, C24, C25</t>
   </si>
   <si>
     <t>100nF</t>
@@ -270,9 +279,6 @@
     <t>490-6213-1-ND</t>
   </si>
   <si>
-    <t>Murata Electronics North America</t>
-  </si>
-  <si>
     <t>GRM1555C1H1R5WA01D</t>
   </si>
   <si>
@@ -345,9 +351,6 @@
     <t>D Zener</t>
   </si>
   <si>
-    <t>Zener Diode</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/texas-instruments/TPD1E10B06DPYR/296-30406-1-ND/3283560</t>
   </si>
   <si>
@@ -372,6 +375,39 @@
     <t>LED1</t>
   </si>
   <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>LED_RX</t>
+  </si>
+  <si>
+    <t>LED RED DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>475-1195-1-ND</t>
+  </si>
+  <si>
+    <t>LS L29K-H1J2-1-Z</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>LED_TX</t>
+  </si>
+  <si>
+    <t>LED YELLOW DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-L29K-H1K2-26-Z/475-1196-1-ND/810357</t>
+  </si>
+  <si>
+    <t>475-1196-1-ND</t>
+  </si>
+  <si>
+    <t>LY L29K-H1K2-26-Z</t>
+  </si>
+  <si>
     <t>E1</t>
   </si>
   <si>
@@ -651,25 +687,28 @@
     <t>ERJ-3GEYJ332V, ERJ-3GEYJ332V, RG1608P-104-B-T5</t>
   </si>
   <si>
-    <t>R5</t>
+    <t>R5, R25, R26</t>
   </si>
   <si>
     <t>1K</t>
   </si>
   <si>
-    <t>RES SMD 1K OHM 0.1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/yageo/RT0603BRD071KL/YAG1237CT-ND/4340590</t>
-  </si>
-  <si>
-    <t>YAG1237CT-ND</t>
-  </si>
-  <si>
-    <t>RT0603BRD071KL</t>
-  </si>
-  <si>
-    <t>R7, R16, R17, R24</t>
+    <t>RES SMD 1K OHM 0.1% 1/10W 0603, RES SMD 1K OHM 1% 1/8W 0603, RES SMD 1K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RT0603BRD071KL/YAG1237CT-ND/4340590, https://www.digikey.com/product-detail/en/vishay-beyschlag/MCT06030C1001FP500/MCT0603-1.00K-CFCT-ND/2607875, https://www.digikey.com/product-detail/en/vishay-beyschlag/MCT06030C1001FP500/MCT0603-1.00K-CFCT-ND/2607875</t>
+  </si>
+  <si>
+    <t>YAG1237CT-ND, MCT0603-1.00K-CFCT-ND, MCT0603-1.00K-CFCT-ND</t>
+  </si>
+  <si>
+    <t>Yageo, Vishay Beyschlag, Vishay Beyschlag</t>
+  </si>
+  <si>
+    <t>RT0603BRD071KL, MCT06030C1001FP500, MCT06030C1001FP500</t>
+  </si>
+  <si>
+    <t>R7, R16, R17, R24, R27</t>
   </si>
   <si>
     <t>0R</t>
@@ -903,7 +942,7 @@
     <t>U3</t>
   </si>
   <si>
-    <t>EFR32BG13P733F512GM48-B</t>
+    <t>EFR32BG13P733F512GM48-C</t>
   </si>
   <si>
     <t>EFR32BG13 Blue Gecko BluetoothÂ® Low Energy SoC</t>
@@ -918,7 +957,25 @@
     <t>Silicon Labs</t>
   </si>
   <si>
-    <t>EFR32BG13P733F512GM48-C</t>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>FT232RL</t>
+  </si>
+  <si>
+    <t>USB Bridge, USB to UART USB 2.0 UART Interface 28-SSOP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/ftdi-future-technology-devices-international-ltd/FT232RL-REEL/768-1007-1-ND/1836402</t>
+  </si>
+  <si>
+    <t>768-1007-1-ND</t>
+  </si>
+  <si>
+    <t>FTDI, Future Technology Devices International Ltd</t>
+  </si>
+  <si>
+    <t>FT232RL-REEL</t>
   </si>
   <si>
     <t>X1</t>
@@ -961,6 +1018,9 @@
   </si>
   <si>
     <t>ECS-.327-12.5-34R-C-TR</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5.5V 14V 2X1SON</t>
   </si>
 </sst>
 </file>
@@ -1343,26 +1403,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC6F85D-366A-410A-AD5D-6C4AE5FB51B3}">
-  <dimension ref="A1:K53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74312339-6D48-4217-93A4-8E4B4ECE47B7}">
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1449,7 +1509,7 @@
         <v>21</v>
       </c>
       <c r="E3" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>23</v>
@@ -1557,71 +1617,71 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
@@ -1630,33 +1690,33 @@
         <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -1665,33 +1725,33 @@
         <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1700,33 +1760,33 @@
         <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1735,33 +1795,33 @@
         <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -1770,33 +1830,33 @@
         <v>23</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E13" s="3">
         <v>2</v>
@@ -1805,30 +1865,30 @@
         <v>23</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
@@ -1840,100 +1900,100 @@
         <v>23</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="K15" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>106</v>
+        <v>331</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
@@ -1945,30 +2005,30 @@
         <v>23</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>14</v>
@@ -1980,30 +2040,30 @@
         <v>23</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>14</v>
@@ -2015,30 +2075,30 @@
         <v>23</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
@@ -2047,33 +2107,33 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>14</v>
@@ -2085,30 +2145,30 @@
         <v>23</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
@@ -2117,176 +2177,176 @@
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>127</v>
+        <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>129</v>
+        <v>14</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="K23" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="3">
-        <v>2</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E27" s="3">
         <v>2</v>
@@ -2295,54 +2355,54 @@
         <v>23</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2356,39 +2416,39 @@
         <v>171</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="E29" s="3">
         <v>2</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>14</v>
@@ -2397,39 +2457,39 @@
         <v>1</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>14</v>
+        <v>178</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>14</v>
+        <v>179</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>14</v>
+        <v>180</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>14</v>
@@ -2452,209 +2512,209 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>179</v>
+        <v>14</v>
       </c>
       <c r="E32" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>181</v>
+        <v>14</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>182</v>
+        <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>184</v>
+        <v>14</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>185</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>187</v>
+        <v>14</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>181</v>
+        <v>14</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>189</v>
+        <v>14</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>190</v>
+        <v>14</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>191</v>
+        <v>14</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E34" s="3">
-        <v>5</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G34" s="2" t="s">
+      <c r="I34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E35" s="3">
-        <v>3</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="I35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" s="3">
+        <v>5</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="I36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E36" s="3">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E37" s="3">
+        <v>3</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E37" s="3">
-        <v>4</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>219</v>
@@ -2674,10 +2734,10 @@
         <v>221</v>
       </c>
       <c r="E38" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>23</v>
+        <v>193</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>223</v>
@@ -2709,7 +2769,7 @@
         <v>228</v>
       </c>
       <c r="E39" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>23</v>
@@ -2724,7 +2784,7 @@
         <v>14</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>232</v>
@@ -2744,7 +2804,7 @@
         <v>234</v>
       </c>
       <c r="E40" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>23</v>
@@ -2759,25 +2819,25 @@
         <v>14</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="E41" s="3">
         <v>1</v>
       </c>
@@ -2785,51 +2845,51 @@
         <v>23</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="E42" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>251</v>
@@ -2846,7 +2906,7 @@
         <v>254</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>14</v>
+        <v>253</v>
       </c>
       <c r="E43" s="3">
         <v>1</v>
@@ -2864,10 +2924,10 @@
         <v>14</v>
       </c>
       <c r="J43" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2881,10 +2941,10 @@
         <v>260</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>14</v>
+        <v>259</v>
       </c>
       <c r="E44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>23</v>
@@ -2902,53 +2962,53 @@
         <v>263</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K45" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="3">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>14</v>
@@ -2960,30 +3020,30 @@
         <v>23</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>14</v>
@@ -2995,135 +3055,135 @@
         <v>23</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E48" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="H48" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="K48" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="I49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E49" s="3">
-        <v>1</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="K49" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="3">
+        <v>10</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E50" s="3">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>14</v>
@@ -3135,89 +3195,194 @@
         <v>23</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>296</v>
+        <v>110</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K52" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" s="3">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J53" s="2" t="s">
+      <c r="K53" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>311</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revision 1 for Schematic Review
</commit_message>
<xml_diff>
--- a/BT Mesh/Project Outputs for BT Mesh/BT Mesh.xlsx
+++ b/BT Mesh/Project Outputs for BT Mesh/BT Mesh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Preshit\Documents\GitHub\Low-Power-Embedded-Design\BT Mesh\Project Outputs for BT Mesh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2FCB981C-BA98-4B5B-A32A-23469D590542}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F9F0D216-0167-4661-9AD3-531228321505}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{1D8F6CD8-5044-47FF-A010-CF7A57ACA4F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{88A5A83A-8F17-40EE-A7BC-310CC9158589}"/>
   </bookViews>
   <sheets>
     <sheet name="BT Mesh" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="335">
   <si>
     <t>Designator</t>
   </si>
@@ -93,22 +93,22 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 25V X7R 0603, CAP CER 1UF 16V X7R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 1UF 25V X5R 0603, CAP CER 0.1UF 25V X7R 0603, CAP CER 0.1UF 25V X7R 0603</t>
+    <t>CAP CER 1UF 16V X7R 0603</t>
   </si>
   <si>
     <t>Digi-Key Link</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM188R71E104KA57D/490-6051-1-ND/3845251, https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B105MO8NNWC/1276-6524-1-ND/5961383, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRT188R61E105ME13D/490-12322-1-ND/5417023, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM188R71E104KA57D/490-6051-1-ND/3845251, https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM188R71E104KA57D/490-6051-1-ND/3845251</t>
-  </si>
-  <si>
-    <t>490-6051-1-ND, 1276-6524-1-ND, 490-12322-1-ND, 490-12322-1-ND, 490-12322-1-ND, 490-6051-1-ND, 490-6051-1-ND</t>
-  </si>
-  <si>
-    <t>Murata Electronics North America, Samsung Electro-Mechanics, Murata Electronics North America, Murata Electronics North America, Murata Electronics North America, Murata Electronics North America, Murata Electronics North America</t>
-  </si>
-  <si>
-    <t>GCM188R71E104KA57D, CL10B105MO8NNWC, GRT188R61E105ME13D, GRT188R61E105ME13D, GRT188R61E105ME13D, GCM188R71E104KA57D, GCM188R71E104KA57D</t>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B105MO8NNWC/1276-6524-1-ND/5961383</t>
+  </si>
+  <si>
+    <t>1276-6524-1-ND</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL10B105MO8NNWC</t>
   </si>
   <si>
     <t>C2, C3, C5, C8, C15</t>
@@ -351,6 +351,9 @@
     <t>D Zener</t>
   </si>
   <si>
+    <t>Zener Diode, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON, TVS DIODE 5.5V 14V 2X1SON</t>
+  </si>
+  <si>
     <t>https://www.digikey.com/product-detail/en/texas-instruments/TPD1E10B06DPYR/296-30406-1-ND/3283560</t>
   </si>
   <si>
@@ -606,9 +609,6 @@
     <t>RES SMD 10K OHM 1% 1/8W 0603</t>
   </si>
   <si>
-    <t>Digi-Key URL</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en?keywords=MCT0603-10.0K-CFCT-ND</t>
   </si>
   <si>
@@ -669,22 +669,19 @@
     <t>100K</t>
   </si>
   <si>
-    <t>RES SMD 3.3K OHM 5% 1/10W 0603, RES SMD 3.3K OHM 5% 1/10W 0603, RES SMD 100K OHM 0.1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>Digi-Key URL, Digi-Key URL, Digi-Key Link</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3GEYJ332V/P3.3KGCT-ND/135146, https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3GEYJ332V/P3.3KGCT-ND/135146, https://www.digikey.com/products/en/resistors/chip-resistor-surface-mount/52?k=RG1608P-104-B-T5&amp;k=&amp;pkeyword=RG1608P-104-B-T5&amp;pv7=2&amp;sf=0&amp;quantity=&amp;ColumnSort=0&amp;page=1&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>P3.3KGCT-ND, P3.3KGCT-ND, RG16P100KBCT-ND</t>
-  </si>
-  <si>
-    <t>Panasonic Electronic Components, Panasonic Electronic Components, Susumu</t>
-  </si>
-  <si>
-    <t>ERJ-3GEYJ332V, ERJ-3GEYJ332V, RG1608P-104-B-T5</t>
+    <t>RES SMD 100K OHM 0.1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en/resistors/chip-resistor-surface-mount/52?k=RG1608P-104-B-T5&amp;k=&amp;pkeyword=RG1608P-104-B-T5&amp;pv7=2&amp;sf=0&amp;quantity=&amp;ColumnSort=0&amp;page=1&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>RG16P100KBCT-ND</t>
+  </si>
+  <si>
+    <t>Susumu</t>
+  </si>
+  <si>
+    <t>RG1608P-104-B-T5</t>
   </si>
   <si>
     <t>R5, R25, R26</t>
@@ -693,19 +690,16 @@
     <t>1K</t>
   </si>
   <si>
-    <t>RES SMD 1K OHM 0.1% 1/10W 0603, RES SMD 1K OHM 1% 1/8W 0603, RES SMD 1K OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/yageo/RT0603BRD071KL/YAG1237CT-ND/4340590, https://www.digikey.com/product-detail/en/vishay-beyschlag/MCT06030C1001FP500/MCT0603-1.00K-CFCT-ND/2607875, https://www.digikey.com/product-detail/en/vishay-beyschlag/MCT06030C1001FP500/MCT0603-1.00K-CFCT-ND/2607875</t>
-  </si>
-  <si>
-    <t>YAG1237CT-ND, MCT0603-1.00K-CFCT-ND, MCT0603-1.00K-CFCT-ND</t>
-  </si>
-  <si>
-    <t>Yageo, Vishay Beyschlag, Vishay Beyschlag</t>
-  </si>
-  <si>
-    <t>RT0603BRD071KL, MCT06030C1001FP500, MCT06030C1001FP500</t>
+    <t>RES SMD 1K OHM 0.1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RT0603BRD071KL/YAG1237CT-ND/4340590</t>
+  </si>
+  <si>
+    <t>YAG1237CT-ND</t>
+  </si>
+  <si>
+    <t>RT0603BRD071KL</t>
   </si>
   <si>
     <t>R7, R16, R17, R24, R27</t>
@@ -816,12 +810,30 @@
     <t>1276-5134-1-ND</t>
   </si>
   <si>
-    <t>Samsung Electro-Mechanics</t>
-  </si>
-  <si>
     <t>RC1608J105CS</t>
   </si>
   <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>PTC FUSE</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 6V 500MA 1206</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/littelfuse-inc/1206L050YR/F2112CT-ND/455721</t>
+  </si>
+  <si>
+    <t>F2112CT-ND</t>
+  </si>
+  <si>
+    <t>Bel Fuse</t>
+  </si>
+  <si>
+    <t>Littelfuse Inc.</t>
+  </si>
+  <si>
     <t>S1</t>
   </si>
   <si>
@@ -1018,9 +1030,6 @@
   </si>
   <si>
     <t>ECS-.327-12.5-34R-C-TR</t>
-  </si>
-  <si>
-    <t>TVS DIODE 5.5V 14V 2X1SON</t>
   </si>
 </sst>
 </file>
@@ -1403,26 +1412,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74312339-6D48-4217-93A4-8E4B4ECE47B7}">
-  <dimension ref="A1:K56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E71A9F0-1271-4C9D-B8E0-03BA3280595F}">
+  <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1993,7 +2002,7 @@
         <v>107</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>331</v>
+        <v>108</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
@@ -2005,27 +2014,27 @@
         <v>23</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>100</v>
@@ -2057,10 +2066,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>100</v>
@@ -2092,13 +2101,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
@@ -2113,7 +2122,7 @@
         <v>101</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>14</v>
@@ -2122,18 +2131,18 @@
         <v>96</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>14</v>
@@ -2145,10 +2154,10 @@
         <v>23</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>14</v>
@@ -2157,18 +2166,18 @@
         <v>96</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
@@ -2197,48 +2206,48 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>14</v>
@@ -2250,34 +2259,34 @@
         <v>23</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
@@ -2285,10 +2294,10 @@
         <v>23</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>14</v>
@@ -2297,22 +2306,22 @@
         <v>33</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E26" s="3">
         <v>1</v>
       </c>
@@ -2320,33 +2329,33 @@
         <v>23</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="E27" s="3">
         <v>2</v>
@@ -2355,10 +2364,10 @@
         <v>23</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>14</v>
@@ -2367,22 +2376,22 @@
         <v>33</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="E28" s="3">
         <v>1</v>
       </c>
@@ -2390,33 +2399,33 @@
         <v>23</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="E29" s="3">
         <v>2</v>
@@ -2425,10 +2434,10 @@
         <v>23</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>14</v>
@@ -2437,53 +2446,53 @@
         <v>33</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>14</v>
@@ -2512,13 +2521,13 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>14</v>
@@ -2547,13 +2556,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>14</v>
@@ -2582,22 +2591,22 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="E34" s="3">
         <v>2</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>193</v>
+        <v>23</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>194</v>
@@ -2632,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>193</v>
+        <v>23</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>201</v>
@@ -2667,7 +2676,7 @@
         <v>5</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>193</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>208</v>
@@ -2702,71 +2711,71 @@
         <v>3</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E38" s="3">
         <v>3</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>193</v>
+        <v>23</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E39" s="3">
         <v>5</v>
@@ -2775,10 +2784,10 @@
         <v>23</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>14</v>
@@ -2787,68 +2796,68 @@
         <v>196</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="D40" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E40" s="3">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="2" t="s">
+      <c r="I40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="D41" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E41" s="3">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>14</v>
@@ -2857,21 +2866,21 @@
         <v>203</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>248</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E42" s="3">
         <v>3</v>
@@ -2880,45 +2889,45 @@
         <v>23</v>
       </c>
       <c r="G42" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E43" s="3">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>14</v>
@@ -2927,21 +2936,21 @@
         <v>203</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E44" s="3">
         <v>2</v>
@@ -2950,439 +2959,474 @@
         <v>23</v>
       </c>
       <c r="G44" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="I45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="3">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G45" s="2" t="s">
+      <c r="K45" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E46" s="3">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G46" s="2" t="s">
+      <c r="I46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="K46" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47" s="3">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G47" s="2" t="s">
+      <c r="I47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="K47" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="D48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E48" s="3">
-        <v>1</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="H48" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J48" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="K48" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="I49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E49" s="3">
-        <v>1</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="2" t="s">
+      <c r="K49" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E50" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="3">
+        <v>10</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E51" s="3">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G51" s="2" t="s">
+      <c r="I51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="K51" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" s="2" t="s">
+      <c r="I52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K52" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" s="3">
-        <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>308</v>
-      </c>
       <c r="I53" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>309</v>
+        <v>111</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" s="3">
-        <v>1</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G54" s="2" t="s">
+      <c r="I54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="H54" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="K54" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="I55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" s="3">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G55" s="2" t="s">
+      <c r="K55" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="H56" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="I56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" s="3">
-        <v>1</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G56" s="2" t="s">
+      <c r="K56" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="H56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>330</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>